<commit_message>
git pie bug and add pie layout
</commit_message>
<xml_diff>
--- a/resources/test_data/hnmftest.xlsx
+++ b/resources/test_data/hnmftest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\zxvis\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74ED024-5505-44EF-A894-E6F23E407583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E938B7-E6C2-4092-A399-EA56E3C2590E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23343" yWindow="-109" windowWidth="23452" windowHeight="12682" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1501" yWindow="1501" windowWidth="23233" windowHeight="12318" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2000" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -575,19 +575,19 @@
         <v>0.2</v>
       </c>
       <c r="D2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="E2">
         <v>0.1</v>
       </c>
       <c r="F2">
-        <v>0.08</v>
+        <v>0.3</v>
       </c>
       <c r="G2">
         <v>0.17</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -601,16 +601,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E3">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="F3">
         <v>0.2</v>
       </c>
       <c r="G3">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="H3">
         <v>0.22</v>
@@ -650,13 +650,13 @@
         <v>0.18</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D5">
         <v>0.18</v>
       </c>
       <c r="E5">
-        <v>0.08</v>
+        <v>0.3</v>
       </c>
       <c r="F5">
         <v>0</v>

</xml_diff>